<commit_message>
Uploaded result and graph
</commit_message>
<xml_diff>
--- a/Dataset/202405-citibike-tripdata_1.xlsx
+++ b/Dataset/202405-citibike-tripdata_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duong\Documents\GitHub\Bike-Sharing-Simulation\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E416933B-4887-4344-B8A0-CA1B96DA0743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6819386-A3C4-4120-BA05-E3228979D94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{AD6143DE-A902-4B58-8481-1850D1AFC164}"/>
+    <workbookView xWindow="2556" yWindow="3012" windowWidth="16440" windowHeight="12120" xr2:uid="{AD6143DE-A902-4B58-8481-1850D1AFC164}"/>
   </bookViews>
   <sheets>
     <sheet name="202405-citibike-tripdata_1" sheetId="1" r:id="rId1"/>
@@ -766,7 +766,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1247,7 +1247,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1295,10 +1295,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="27" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="yyyy/mm/dd\ h:mm"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1652,13 +1652,13 @@
   <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
@@ -1669,10 +1669,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">

</xml_diff>